<commit_message>
update link video clase 3
</commit_message>
<xml_diff>
--- a/clase_03/input/ejemplo_1.xlsx
+++ b/clase_03/input/ejemplo_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calle 11 Hostel\Desktop\Projectos eduard\taller_cief_202102\clase_03\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduard-martinez/Dropbox/teaching/r_cief/taller_cief_202102/clase_03/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4EA53B9-D8DA-427E-82BB-BC822D39790F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7160A2-CF1C-EE49-BD55-E3C32A67A836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22905" yWindow="2595" windowWidth="29040" windowHeight="15840" xr2:uid="{323DA0C2-F2B6-4CAC-8F44-E284E34D3E25}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{323DA0C2-F2B6-4CAC-8F44-E284E34D3E25}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>sexo</t>
   </si>
@@ -403,15 +403,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE9739A-1724-4DDA-BB53-0D000D3F1E50}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -422,58 +422,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>101</v>
       </c>
       <c r="B2" s="1">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>201</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>101</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>201</v>
       </c>
       <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>301</v>
+      </c>
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>201</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>301</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>